<commit_message>
changed story file internal structure
</commit_message>
<xml_diff>
--- a/Assets/Stories.xlsx
+++ b/Assets/Stories.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\visualstudio workstation\TheMoneyIsAlwaysRight\TheMoneyIsAlwaysRight\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E28B667-28AF-4807-8D08-997967CF0337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3372DF53-8F12-4EB1-BFBE-438B231C1669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2850" yWindow="2895" windowWidth="21600" windowHeight="11385" xr2:uid="{2B3A7A2A-41FE-48F0-8011-C13D9C1E3496}"/>
+    <workbookView xWindow="9480" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{2B3A7A2A-41FE-48F0-8011-C13D9C1E3496}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,68 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
-  <si>
-    <t>#SOS1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>#EOS1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>#EOF</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>#EOS2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>#SOS2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>#SOS3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>#EOS3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>#SOS4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>#EOS4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>#SOS5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>#EOS5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>#SOS6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>#EOS6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>#EOS7</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>#SOS7</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>스토리 1-1. 앞으로 진행한다</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -123,6 +67,86 @@
   </si>
   <si>
     <t>스토리 2-4. 이전으로 돌아간다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#SOS1-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#EOS1-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#SOS1-2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#EOS1-2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#SOS1-3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#EOS1-3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#SOS2-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#EOS2-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#SOS2-2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#EOS2-2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#SOS2-3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#EOS2-3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#SOS2-4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#EOS2-4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#SOS0-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#EOS0-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스토리 0-1. 1을 눌러 게임 시작</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#SOS0-0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#EOS0-0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 : 진행, 2 : 게임 엔딩 , 3:현제에 머무른다</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -507,122 +531,152 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8226566C-F20D-40E4-813F-125FF91969D3}">
-  <dimension ref="A1:A22"/>
+  <dimension ref="A1:A28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>2</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>